<commit_message>
Uploaded CSV Removed Videos and Illustrations from Shop
</commit_message>
<xml_diff>
--- a/public/static/assets/LuupeMarketplaceUploadTemplate.xlsx
+++ b/public/static/assets/LuupeMarketplaceUploadTemplate.xlsx
@@ -4,20 +4,15 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Images" sheetId="1" r:id="rId4"/>
-    <sheet state="hidden" name="Options" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Options" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="Bo84wzdI9TMHMbBZ6XQO3m9nm7EkVFBGPR6uFVWfNd0="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>File Name</t>
   </si>
@@ -73,9 +68,6 @@
     <t>Illustration</t>
   </si>
   <si>
-    <t>Post-event</t>
-  </si>
-  <si>
     <t>Business &amp; Technology</t>
   </si>
   <si>
@@ -85,10 +77,16 @@
     <t>Food &amp; Drink</t>
   </si>
   <si>
+    <t>Health &amp; Wellness</t>
+  </si>
+  <si>
     <t>Arts &amp; Culture</t>
   </si>
   <si>
     <t>Sports &amp; Recreation</t>
+  </si>
+  <si>
+    <t>Science &amp; Education</t>
   </si>
   <si>
     <t>Fashion &amp; Beauty</t>
@@ -104,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -126,12 +124,16 @@
     <font>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -143,8 +145,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF666666"/>
-        <bgColor rgb="FF666666"/>
+        <fgColor rgb="FF434343"/>
+        <bgColor rgb="FF434343"/>
       </patternFill>
     </fill>
   </fills>
@@ -160,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -168,7 +170,7 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
@@ -179,6 +181,12 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1726,7 +1734,7 @@
       <formula1>Options!$G$1:$G$2</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E16">
-      <formula1>Options!$C$1:$C$11</formula1>
+      <formula1>Options!$C$1:$C$12</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F16">
       <formula1>Options!$E$1:$E$2</formula1>
@@ -1759,7 +1767,7 @@
       <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="7" t="s">
@@ -1773,7 +1781,7 @@
       <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -1787,51 +1795,55 @@
       <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="C12" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="13" ht="15.75" customHeight="1"/>
     <row r="14" ht="15.75" customHeight="1"/>
     <row r="15" ht="15.75" customHeight="1"/>

</xml_diff>